<commit_message>
fixed historical_angel to start actually from fromdate n end at todate
</commit_message>
<xml_diff>
--- a/research/1yr/stock-returns-1yr-2023-01-15.xlsx
+++ b/research/1yr/stock-returns-1yr-2023-01-15.xlsx
@@ -1128,23 +1128,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -1153,23 +1136,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J322"/>
+  <dimension ref="A1:K322"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.66"/>
   </cols>
   <sheetData>
@@ -1233,6 +1216,9 @@
       <c r="J2" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K2" s="0" t="n">
+        <v>24.65</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
@@ -1265,6 +1251,9 @@
       <c r="J3" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K3" s="0" t="n">
+        <v>236</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="n">
@@ -1297,6 +1286,9 @@
       <c r="J4" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K4" s="0" t="n">
+        <v>97.7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -1329,6 +1321,9 @@
       <c r="J5" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K5" s="0" t="n">
+        <v>570</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -1361,6 +1356,9 @@
       <c r="J6" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K6" s="0" t="n">
+        <v>157</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -1393,6 +1391,9 @@
       <c r="J7" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K7" s="0" t="n">
+        <v>272</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -1425,6 +1426,9 @@
       <c r="J8" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K8" s="0" t="n">
+        <v>640</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -1457,6 +1461,9 @@
       <c r="J9" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K9" s="0" t="n">
+        <v>1405</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -1489,6 +1496,9 @@
       <c r="J10" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K10" s="0" t="n">
+        <v>3989</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -1521,6 +1531,9 @@
       <c r="J11" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K11" s="0" t="n">
+        <v>1294</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -1552,6 +1565,9 @@
       </c>
       <c r="J12" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>392</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1585,6 +1601,9 @@
       <c r="J13" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K13" s="0" t="n">
+        <v>67.75</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -1617,6 +1636,9 @@
       <c r="J14" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K14" s="0" t="n">
+        <v>70.15</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -1649,6 +1671,9 @@
       <c r="J15" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K15" s="0" t="n">
+        <v>1727</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -1681,6 +1706,9 @@
       <c r="J16" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K16" s="0" t="n">
+        <v>390</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -1713,6 +1741,9 @@
       <c r="J17" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K17" s="0" t="n">
+        <v>319</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -1745,6 +1776,9 @@
       <c r="J18" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K18" s="0" t="n">
+        <v>44.35</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1777,6 +1811,9 @@
       <c r="J19" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K19" s="0" t="n">
+        <v>25.4</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -1809,6 +1846,9 @@
       <c r="J20" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="K20" s="0" t="n">
+        <v>24.2</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -1840,6 +1880,9 @@
       </c>
       <c r="J21" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>357</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>